<commit_message>
changed max HnS block size from 390 to 490
</commit_message>
<xml_diff>
--- a/LargeScaleHnS.xlsx
+++ b/LargeScaleHnS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsofteur-my.sharepoint.com/personal/jomore_microsoft_com/Documents/Customers/Atruvia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1232" documentId="8_{AB7DC771-E95C-4CC1-8C4E-CBE3B24F299A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51F295F8-BFEE-4D40-9E41-F0A5AEE8CB98}"/>
+  <xr:revisionPtr revIDLastSave="1240" documentId="8_{AB7DC771-E95C-4CC1-8C4E-CBE3B24F299A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05B2209D-9818-487B-BA68-8B42FE7CF001}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{4585D9A0-E3B1-493C-9DE6-E504132A0FCE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4585D9A0-E3B1-493C-9DE6-E504132A0FCE}"/>
   </bookViews>
   <sheets>
     <sheet name="AzNWDesign" sheetId="1" r:id="rId1"/>
@@ -725,9 +725,6 @@
     <t>Last edited</t>
   </si>
   <si>
-    <t>Jan 19th 2026</t>
-  </si>
-  <si>
     <t>Jose Moreno</t>
   </si>
   <si>
@@ -738,6 +735,9 @@
   </si>
   <si>
     <t>Azure pricing (monthly, USD), last updated in Jan 26</t>
+  </si>
+  <si>
+    <t>Jan 23rd 2026</t>
   </si>
 </sst>
 </file>
@@ -848,10 +848,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2205,50 +2205,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>12611</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>1440437</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E03420DE-06AB-D359-CB9B-A2797F2EF902}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8004086" y="4000501"/>
-          <a:ext cx="8733501" cy="4772024"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>78</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -2273,7 +2229,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2282,6 +2238,50 @@
         <a:xfrm>
           <a:off x="8010525" y="14458950"/>
           <a:ext cx="7742111" cy="4886325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>598284</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>981201</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0B2AFC3-3FE9-9E8A-60C7-0A2CBA806F08}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8313534" y="4400549"/>
+          <a:ext cx="8298192" cy="4562475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2616,29 +2616,29 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.453125" customWidth="1"/>
-    <col min="2" max="2" width="19.54296875" customWidth="1"/>
-    <col min="3" max="3" width="19.453125" customWidth="1"/>
-    <col min="4" max="4" width="22.54296875" customWidth="1"/>
-    <col min="5" max="5" width="19.7265625" customWidth="1"/>
-    <col min="7" max="7" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7265625" customWidth="1"/>
-    <col min="11" max="11" width="12.81640625" customWidth="1"/>
-    <col min="14" max="14" width="35.1796875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="31" x14ac:dyDescent="0.7">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>74</v>
@@ -2647,12 +2647,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>38</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>1</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>39</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>2</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>6</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>1570.23</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>7</v>
       </c>
@@ -2756,49 +2756,49 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B12">
         <v>182.5</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="E12" s="10"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B13">
         <v>73</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B14">
         <v>0.02</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B15">
         <v>306.60000000000002</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>37</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>36.5</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>12</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>13</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>14</v>
       </c>
@@ -2833,13 +2833,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="E21" s="1"/>
       <c r="H21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>20</v>
       </c>
@@ -2856,7 +2856,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -2877,12 +2877,12 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
       <c r="B24">
-        <v>390</v>
+        <v>490</v>
       </c>
       <c r="C24">
         <v>590</v>
@@ -2894,7 +2894,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>65</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -2979,7 +2979,7 @@
       </c>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>17</v>
       </c>
@@ -3002,7 +3002,7 @@
       <c r="I29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -3025,7 +3025,7 @@
       <c r="I30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -3047,7 +3047,7 @@
       </c>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -3070,7 +3070,7 @@
       <c r="I32" s="4"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -3092,7 +3092,7 @@
       </c>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -3114,7 +3114,7 @@
       </c>
       <c r="L34" s="1"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -3156,7 +3156,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>55</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>912.5</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>56</v>
       </c>
@@ -3199,7 +3199,7 @@
       </c>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -3218,7 +3218,7 @@
       </c>
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -3240,7 +3240,7 @@
       </c>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -3280,7 +3280,7 @@
       <c r="I42" s="1"/>
       <c r="L42" s="1"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -3299,7 +3299,7 @@
       </c>
       <c r="L43" s="1"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -3320,7 +3320,7 @@
       <c r="I44" s="1"/>
       <c r="L44" s="1"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
@@ -3342,7 +3342,7 @@
       </c>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -3363,7 +3363,7 @@
         <v>3.0864197530864196E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -3385,7 +3385,7 @@
       </c>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -3405,7 +3405,7 @@
       </c>
       <c r="I48" s="3"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>263.52999999999997</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>68</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>70</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>69</v>
       </c>
@@ -3483,7 +3483,7 @@
       </c>
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>49</v>
       </c>
@@ -3502,7 +3502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>50</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>263.52999999999997</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>51</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>52</v>
       </c>
@@ -3561,7 +3561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>53</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>18</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>2934.6</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>54</v>
       </c>
@@ -3617,7 +3617,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>17</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>119.60000000000002</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>944.5</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>58</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>57</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>263.52999999999997</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>53</v>
       </c>
@@ -3722,7 +3722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>18</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>2949.2</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>33</v>
       </c>
@@ -3761,7 +3761,7 @@
         <v>4276.83</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G79" s="1" t="s">
         <v>63</v>
       </c>
@@ -3801,37 +3801,37 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>79</v>
       </c>
       <c r="B1">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
       <c r="B2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>